<commit_message>
Updated pub and conferences
Updated biblo details for Yeo, Pollack, Merkley, Ansari, & Price (2020), and updated cancellation of 2020 conferences due to COVID-19
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djyeo/Google Drive/cv/yeodj-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D7AEBC-200E-E14F-A953-76EFC1477E05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06EEA3D-64B0-5443-B28B-5FEFAB262B1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8080" yWindow="460" windowWidth="20400" windowHeight="16660" xr2:uid="{9662CE4C-DEF8-8749-ABE3-ABD9C0AA9720}"/>
+    <workbookView xWindow="2020" yWindow="460" windowWidth="26460" windowHeight="16660" xr2:uid="{9662CE4C-DEF8-8749-ABE3-ABD9C0AA9720}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="198">
   <si>
     <t>authors</t>
   </si>
@@ -297,18 +297,12 @@
     <t xml:space="preserve">Conrad, B., Wilkey, E. D., Yeo, D. J., &amp; Price, G. R. </t>
   </si>
   <si>
-    <t>Pillai, R. M., Loehr, A., Yeo, D. J., Hong, C., Rittle-Johnson, B., &amp; Fazio, L. K.</t>
-  </si>
-  <si>
     <t>Network topology of symbolic and nonsymbolic number comparison</t>
   </si>
   <si>
     <t>The "Inferior Temporal Numeral Area" distinguishes numerals from other character categories during passive viewing: A representational similarity analysis</t>
   </si>
   <si>
-    <t>Are there Costs to using Incorrect Worked Examples in Mathematics Education?</t>
-  </si>
-  <si>
     <t>Primary Mathematics (2021 Edition) Student Book 2A</t>
   </si>
   <si>
@@ -603,7 +597,28 @@
     <t>Singaporean Researchers Global Summit</t>
   </si>
   <si>
-    <t>in press</t>
+    <t>May, 2020</t>
+  </si>
+  <si>
+    <t>“Number form area” distinguishes between numerals and other character categories during passive viewing: A meta-synthesis of representational similarity analyses with three studies</t>
+  </si>
+  <si>
+    <t>Vision Sciences Society</t>
+  </si>
+  <si>
+    <t>St. Pete Beach, FL, USA</t>
+  </si>
+  <si>
+    <t>cancelled</t>
+  </si>
+  <si>
+    <t>June, 2020</t>
+  </si>
+  <si>
+    <t>Representational distinction of numbers, letters, and novel characters in the “number form area”</t>
+  </si>
+  <si>
+    <t>Montreal, QC, Canada</t>
   </si>
 </sst>
 </file>
@@ -989,18 +1004,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF752879-4E41-3C4A-A16F-F1C105CAD07B}">
-  <dimension ref="A1:V41"/>
+  <dimension ref="A1:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="104.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="146.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="127.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60.83203125" customWidth="1"/>
     <col min="7" max="8" width="10.83203125" customWidth="1"/>
     <col min="9" max="9" width="12.1640625" customWidth="1"/>
@@ -1013,7 +1028,7 @@
     <col min="19" max="20" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1069,10 +1084,10 @@
         <v>22</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>23</v>
@@ -1080,8 +1095,11 @@
       <c r="V1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="17">
+      <c r="W1" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="17">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1091,23 +1109,27 @@
       <c r="C2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>192</v>
+      <c r="D2" s="1">
+        <v>2020</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1">
+        <v>213</v>
+      </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1">
+        <v>116716</v>
+      </c>
       <c r="J2" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1118,12 +1140,12 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
     </row>
-    <row r="3" spans="1:22" ht="17">
+    <row r="3" spans="1:23" ht="17">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1160,11 +1182,11 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="U3" s="1"/>
     </row>
-    <row r="4" spans="1:22" ht="17">
+    <row r="4" spans="1:23" ht="17">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1209,7 +1231,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="1:22" ht="17">
+    <row r="5" spans="1:23" ht="17">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1252,7 +1274,7 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="1:22" ht="17">
+    <row r="6" spans="1:23" ht="17">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1294,12 +1316,12 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="T6" s="5"/>
       <c r="U6" s="1"/>
     </row>
-    <row r="7" spans="1:22" ht="17">
+    <row r="7" spans="1:23" ht="17">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1342,7 +1364,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="1:22" ht="17">
+    <row r="8" spans="1:23" ht="17">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1387,7 +1409,7 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="1:22" ht="17">
+    <row r="9" spans="1:23" ht="17">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1432,7 +1454,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="1:22" ht="17">
+    <row r="10" spans="1:23" ht="17">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1477,7 +1499,7 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="1:22" ht="17">
+    <row r="11" spans="1:23" ht="17">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1517,12 +1539,12 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="T11" s="5"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="1:22" ht="17">
+    <row r="12" spans="1:23" ht="17">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1567,7 +1589,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="1:22" ht="17">
+    <row r="13" spans="1:23" ht="17">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1575,16 +1597,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D13" s="1">
         <v>2008</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -1593,11 +1615,11 @@
         <v>1</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -1610,21 +1632,21 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="1:22" ht="17">
+    <row r="14" spans="1:23" ht="17">
       <c r="A14" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1643,30 +1665,32 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:22" ht="17">
+    <row r="15" spans="1:23">
       <c r="A15" s="1" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>93</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="2"/>
+      <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>169</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1676,18 +1700,18 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:23">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1697,10 +1721,10 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1711,18 +1735,18 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:23">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1732,10 +1756,10 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1746,18 +1770,18 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:23">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>187</v>
+        <v>168</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2014</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1767,10 +1791,10 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1781,15 +1805,15 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:23">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>170</v>
+        <v>97</v>
       </c>
       <c r="D19" s="1">
         <v>2014</v>
@@ -1802,10 +1826,10 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1816,56 +1840,65 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:23">
       <c r="A20" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>110</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q20" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="W20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1">
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>114</v>
+        <v>191</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1876,13 +1909,13 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="O21" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>140</v>
+        <v>193</v>
       </c>
       <c r="Q21" s="1" t="b">
         <v>1</v>
@@ -1891,8 +1924,11 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="W21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1900,13 +1936,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1917,37 +1953,40 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="O22" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="Q22" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
-    </row>
-    <row r="23" spans="1:22" ht="17">
+      <c r="W22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1">
         <v>4</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>29</v>
+      <c r="C23" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>103</v>
+        <v>181</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -1958,40 +1997,40 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1" t="s">
-        <v>104</v>
+        <v>189</v>
       </c>
       <c r="O23" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>105</v>
+        <v>160</v>
       </c>
       <c r="Q23" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
-      <c r="V23" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="W23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="17">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="1">
         <v>5</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>107</v>
+      <c r="C24" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -2002,26 +2041,29 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="O24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="Q24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
       <c r="V24" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22">
+        <v>104</v>
+      </c>
+      <c r="W24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" s="1" t="s">
         <v>15</v>
       </c>
@@ -2029,13 +2071,13 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -2046,23 +2088,29 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="O25" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="Q25" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
-    </row>
-    <row r="26" spans="1:22">
+      <c r="V25" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="W25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
@@ -2070,13 +2118,13 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -2087,23 +2135,26 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="O26" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="Q26" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
-    </row>
-    <row r="27" spans="1:22">
+      <c r="W26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -2111,13 +2162,13 @@
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -2128,13 +2179,13 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="O27" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="Q27" s="1" t="b">
         <v>0</v>
@@ -2143,8 +2194,11 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
-    </row>
-    <row r="28" spans="1:22">
+      <c r="W27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -2152,13 +2206,13 @@
         <v>9</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>121</v>
+        <v>33</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -2169,23 +2223,26 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O28" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="Q28" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
-    </row>
-    <row r="29" spans="1:22">
+      <c r="W28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
       <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
@@ -2193,13 +2250,13 @@
         <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -2210,13 +2267,13 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O29" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="Q29" s="1" t="b">
         <v>1</v>
@@ -2225,8 +2282,11 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
-    </row>
-    <row r="30" spans="1:22">
+      <c r="W29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -2234,13 +2294,13 @@
         <v>11</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2251,13 +2311,13 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="O30" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="Q30" s="1" t="b">
         <v>1</v>
@@ -2266,8 +2326,11 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
-    </row>
-    <row r="31" spans="1:22">
+      <c r="W30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
       <c r="A31" s="1" t="s">
         <v>15</v>
       </c>
@@ -2275,13 +2338,13 @@
         <v>12</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>132</v>
+        <v>28</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -2292,13 +2355,13 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="O31" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="Q31" s="1" t="b">
         <v>1</v>
@@ -2307,8 +2370,11 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
-    </row>
-    <row r="32" spans="1:22" ht="17">
+      <c r="W31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
       <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
@@ -2316,13 +2382,13 @@
         <v>13</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -2333,13 +2399,13 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="O32" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="Q32" s="1" t="b">
         <v>1</v>
@@ -2348,10 +2414,13 @@
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
-    </row>
-    <row r="33" spans="1:21">
+      <c r="W32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="17">
       <c r="A33" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B33" s="1">
         <v>14</v>
@@ -2360,10 +2429,10 @@
         <v>33</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -2374,13 +2443,13 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="O33" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="Q33" s="1" t="b">
         <v>1</v>
@@ -2389,10 +2458,13 @@
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
-    </row>
-    <row r="34" spans="1:21">
+      <c r="W33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
       <c r="A34" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B34" s="1">
         <v>15</v>
@@ -2401,10 +2473,10 @@
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -2415,23 +2487,26 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="O34" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="Q34" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
-    </row>
-    <row r="35" spans="1:21">
+      <c r="W34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23">
       <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
@@ -2439,13 +2514,13 @@
         <v>16</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -2456,25 +2531,26 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="O35" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="Q35" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="R35" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="S35" s="5"/>
-      <c r="T35" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
       <c r="U35" s="1"/>
-    </row>
-    <row r="36" spans="1:21">
+      <c r="W35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23">
       <c r="A36" s="1" t="s">
         <v>15</v>
       </c>
@@ -2482,13 +2558,13 @@
         <v>17</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>33</v>
+        <v>140</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>20</v>
+        <v>141</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -2499,23 +2575,28 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="O36" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="Q36" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="R36" s="1"/>
-      <c r="S36" s="1"/>
-      <c r="T36" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="R36" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
       <c r="U36" s="1"/>
-    </row>
-    <row r="37" spans="1:21">
+      <c r="W36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
@@ -2523,13 +2604,13 @@
         <v>18</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>150</v>
+        <v>33</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>151</v>
+        <v>20</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -2540,23 +2621,26 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="O37" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="Q37" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
-    </row>
-    <row r="38" spans="1:21">
+      <c r="W37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23">
       <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
@@ -2564,13 +2648,13 @@
         <v>19</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -2581,13 +2665,13 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="O38" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Q38" s="1" t="b">
         <v>1</v>
@@ -2596,8 +2680,11 @@
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
-    </row>
-    <row r="39" spans="1:21">
+      <c r="W38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23">
       <c r="A39" s="1" t="s">
         <v>15</v>
       </c>
@@ -2605,13 +2692,13 @@
         <v>20</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -2622,39 +2709,40 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="O39" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="Q39" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="R39" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
       <c r="U39" s="1"/>
-    </row>
-    <row r="40" spans="1:21">
+      <c r="W39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23">
       <c r="A40" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B40" s="1">
         <v>21</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -2665,37 +2753,42 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O40" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="Q40" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="R40" s="1"/>
-      <c r="S40" s="1"/>
-      <c r="T40" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="R40" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
       <c r="U40" s="1"/>
-    </row>
-    <row r="41" spans="1:21">
+      <c r="W40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23">
       <c r="A41" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B41" s="1">
         <v>22</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>65</v>
+        <v>159</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>165</v>
+        <v>21</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -2706,13 +2799,13 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="O41" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="Q41" s="1" t="b">
         <v>0</v>
@@ -2721,16 +2814,63 @@
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
+      <c r="W41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23">
+      <c r="A42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="1">
+        <v>23</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="O42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q42" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="W42" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1" xr:uid="{EA8BD15C-A187-764A-953D-0D17A1C363EA}"/>
     <hyperlink ref="K6" r:id="rId2" xr:uid="{79CF63DC-6383-1741-BF3D-C33FDC6CE3BA}"/>
-    <hyperlink ref="V23" r:id="rId3" xr:uid="{7E24366A-48CB-BA48-A05E-04CB0A830D88}"/>
-    <hyperlink ref="R35" r:id="rId4" xr:uid="{BD7B75BD-10E6-D042-BB4B-B9FECE5F4A72}"/>
-    <hyperlink ref="R39" r:id="rId5" xr:uid="{7233F9C9-C8FD-964A-B5D5-A5817B6795E6}"/>
-    <hyperlink ref="V24" r:id="rId6" xr:uid="{2A8EACE2-271D-3249-86ED-EF7E8BCD613A}"/>
+    <hyperlink ref="V24" r:id="rId3" xr:uid="{7E24366A-48CB-BA48-A05E-04CB0A830D88}"/>
+    <hyperlink ref="R36" r:id="rId4" xr:uid="{BD7B75BD-10E6-D042-BB4B-B9FECE5F4A72}"/>
+    <hyperlink ref="R40" r:id="rId5" xr:uid="{7233F9C9-C8FD-964A-B5D5-A5817B6795E6}"/>
+    <hyperlink ref="V25" r:id="rId6" xr:uid="{2A8EACE2-271D-3249-86ED-EF7E8BCD613A}"/>
     <hyperlink ref="K13" r:id="rId7" xr:uid="{14FB4927-F8C4-4C4C-AB07-BB3E227B7A01}"/>
     <hyperlink ref="S11" r:id="rId8" xr:uid="{F42E1E3D-AF71-4F45-9056-E81407BDCEF5}"/>
     <hyperlink ref="S6" r:id="rId9" xr:uid="{D6AAB031-B949-2944-AD63-AA98423BAE4B}"/>

</xml_diff>

<commit_message>
Removed month as journal's issue#
</commit_message>
<xml_diff>
--- a/data/pubs.xlsx
+++ b/data/pubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djyeo/Google Drive/cv/yeodj-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06EEA3D-64B0-5443-B28B-5FEFAB262B1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ADA3A8-3E76-8B46-9E04-9B6837F23F8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2020" yWindow="460" windowWidth="26460" windowHeight="16660" xr2:uid="{9662CE4C-DEF8-8749-ABE3-ABD9C0AA9720}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="194">
   <si>
     <t>authors</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Acta Psychologica</t>
   </si>
   <si>
-    <t>June</t>
-  </si>
-  <si>
     <t>10.1016/j.actpsy.2019.102877</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>﻿https://linkinghub.elsevier.com/retrieve/pii/S0149763417300325</t>
   </si>
   <si>
-    <t>July</t>
-  </si>
-  <si>
     <t>Price, G. R., Wilkey, E. D., &amp; Yeo, D. J.</t>
   </si>
   <si>
@@ -237,9 +231,6 @@
     <t>﻿https://linkinghub.elsevier.com/retrieve/pii/S0001691816302025</t>
   </si>
   <si>
-    <t>May</t>
-  </si>
-  <si>
     <t>The relation between 1st grade grey matter volume and 2nd grade math competence</t>
   </si>
   <si>
@@ -250,9 +241,6 @@
   </si>
   <si>
     <t>﻿https://linkinghub.elsevier.com/retrieve/pii/S105381191500765X</t>
-  </si>
-  <si>
-    <t>January</t>
   </si>
   <si>
     <t>A metacognitive-based instruction for Primary Four studentsto approach non-routine mathematical word problems</t>
@@ -1007,8 +995,8 @@
   <dimension ref="A1:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1084,10 +1072,10 @@
         <v>22</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>23</v>
@@ -1096,7 +1084,7 @@
         <v>26</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="17">
@@ -1107,16 +1095,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1">
         <v>2020</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G2" s="1">
         <v>213</v>
@@ -1126,10 +1114,10 @@
         <v>116716</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1140,7 +1128,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
@@ -1182,7 +1170,7 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="U3" s="1"/>
     </row>
@@ -1208,17 +1196,15 @@
       <c r="G4" s="1">
         <v>198</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="1">
         <v>102877</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1239,29 +1225,29 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1">
         <v>2019</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="G5" s="1">
         <v>7</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -1282,16 +1268,16 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1">
         <v>2019</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="G6" s="1">
         <v>111</v>
@@ -1300,13 +1286,13 @@
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -1316,7 +1302,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="T6" s="5"/>
       <c r="U6" s="1"/>
@@ -1329,29 +1315,29 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1">
         <v>2018</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="G7" s="1">
         <v>30</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1378,25 +1364,23 @@
         <v>2017</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="G8" s="1">
         <v>78</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>62</v>
-      </c>
+      <c r="H8" s="6"/>
       <c r="I8" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -1417,13 +1401,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D9" s="1">
         <v>2017</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>36</v>
@@ -1431,17 +1415,15 @@
       <c r="G9" s="1">
         <v>176</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -1462,31 +1444,29 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D10" s="1">
         <v>2016</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G10" s="1">
         <v>124</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1507,29 +1487,29 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D11" s="1">
         <v>2014</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G11" s="1">
         <v>46</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1539,7 +1519,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="T11" s="5"/>
       <c r="U11" s="1"/>
@@ -1552,13 +1532,13 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D12" s="1">
         <v>2010</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>36</v>
@@ -1570,13 +1550,13 @@
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1597,16 +1577,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D13" s="1">
         <v>2008</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -1615,11 +1595,11 @@
         <v>1</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -1634,19 +1614,19 @@
     </row>
     <row r="14" spans="1:23" ht="17">
       <c r="A14" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1673,10 +1653,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1686,10 +1666,10 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1708,10 +1688,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1721,10 +1701,10 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1743,10 +1723,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1756,10 +1736,10 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1778,7 +1758,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D18" s="1">
         <v>2014</v>
@@ -1791,10 +1771,10 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1813,7 +1793,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D19" s="1">
         <v>2014</v>
@@ -1826,10 +1806,10 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1848,13 +1828,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1865,13 +1845,13 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O20" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="Q20" s="1" t="b">
         <v>1</v>
@@ -1892,13 +1872,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1909,13 +1889,13 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="O21" s="1" t="b">
         <v>0</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="Q21" s="1" t="b">
         <v>1</v>
@@ -1936,13 +1916,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1953,13 +1933,13 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="O22" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="Q22" s="1" t="b">
         <v>1</v>
@@ -1980,13 +1960,13 @@
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -1997,13 +1977,13 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="O23" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="Q23" s="1" t="b">
         <v>0</v>
@@ -2027,10 +2007,10 @@
         <v>29</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -2041,13 +2021,13 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="O24" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="Q24" s="1" t="b">
         <v>1</v>
@@ -2057,7 +2037,7 @@
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
       <c r="V24" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="W24" t="b">
         <v>0</v>
@@ -2071,13 +2051,13 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -2088,13 +2068,13 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="O25" s="1" t="b">
         <v>0</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="Q25" s="1" t="b">
         <v>0</v>
@@ -2104,7 +2084,7 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
       <c r="V25" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="W25" t="b">
         <v>0</v>
@@ -2118,13 +2098,13 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -2135,13 +2115,13 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O26" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="Q26" s="1" t="b">
         <v>1</v>
@@ -2179,13 +2159,13 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="O27" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q27" s="1" t="b">
         <v>0</v>
@@ -2212,7 +2192,7 @@
         <v>27</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -2223,13 +2203,13 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="O28" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="Q28" s="1" t="b">
         <v>0</v>
@@ -2250,13 +2230,13 @@
         <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -2267,13 +2247,13 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="O29" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="Q29" s="1" t="b">
         <v>1</v>
@@ -2294,13 +2274,13 @@
         <v>11</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2311,13 +2291,13 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="O30" s="1" t="b">
         <v>0</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="Q30" s="1" t="b">
         <v>1</v>
@@ -2344,7 +2324,7 @@
         <v>28</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -2355,13 +2335,13 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O31" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="Q31" s="1" t="b">
         <v>1</v>
@@ -2382,13 +2362,13 @@
         <v>13</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -2399,13 +2379,13 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="O32" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="Q32" s="1" t="b">
         <v>1</v>
@@ -2429,10 +2409,10 @@
         <v>33</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -2443,13 +2423,13 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="O33" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Q33" s="1" t="b">
         <v>1</v>
@@ -2473,10 +2453,10 @@
         <v>33</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -2487,13 +2467,13 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O34" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="Q34" s="1" t="b">
         <v>1</v>
@@ -2517,10 +2497,10 @@
         <v>33</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -2531,13 +2511,13 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="O35" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="Q35" s="1" t="b">
         <v>0</v>
@@ -2558,13 +2538,13 @@
         <v>17</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -2575,19 +2555,19 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O36" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="Q36" s="1" t="b">
         <v>1</v>
       </c>
       <c r="R36" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
@@ -2610,7 +2590,7 @@
         <v>20</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -2621,13 +2601,13 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="O37" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="Q37" s="1" t="b">
         <v>0</v>
@@ -2648,13 +2628,13 @@
         <v>19</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -2665,13 +2645,13 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="O38" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="Q38" s="1" t="b">
         <v>1</v>
@@ -2692,13 +2672,13 @@
         <v>20</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -2709,13 +2689,13 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O39" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="Q39" s="1" t="b">
         <v>1</v>
@@ -2736,13 +2716,13 @@
         <v>21</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -2753,19 +2733,19 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="O40" s="1" t="b">
         <v>0</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="Q40" s="1" t="b">
         <v>1</v>
       </c>
       <c r="R40" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
@@ -2782,13 +2762,13 @@
         <v>22</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -2799,13 +2779,13 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O41" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="Q41" s="1" t="b">
         <v>0</v>
@@ -2826,13 +2806,13 @@
         <v>23</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -2843,13 +2823,13 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="O42" s="1" t="b">
         <v>1</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="Q42" s="1" t="b">
         <v>0</v>

</xml_diff>